<commit_message>
chore(doc): update import docs
</commit_message>
<xml_diff>
--- a/packages/app/public/static/docs/Template_import_mesures.xlsx
+++ b/packages/app/public/static/docs/Template_import_mesures.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>date_ouverture</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>75002</t>
+  </si>
+  <si>
+    <t>antenne</t>
+  </si>
+  <si>
+    <t>MONTREUIL</t>
   </si>
 </sst>
 </file>
@@ -77,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -110,7 +116,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -460,7 +466,7 @@
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,8 +497,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>43820</v>
       </c>
@@ -519,6 +528,9 @@
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(import): update headers and import async (#1603)
* fix(import): add antenne column

* chore(doc): update import docs

* feat(import): import mesure asynchronously

* feat(import): update counter states

* fix(import): fix antenne association
</commit_message>
<xml_diff>
--- a/packages/app/public/static/docs/Template_import_mesures.xlsx
+++ b/packages/app/public/static/docs/Template_import_mesures.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>date_ouverture</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>75002</t>
+  </si>
+  <si>
+    <t>antenne</t>
+  </si>
+  <si>
+    <t>MONTREUIL</t>
   </si>
 </sst>
 </file>
@@ -77,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -110,7 +116,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -460,7 +466,7 @@
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,8 +497,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>43820</v>
       </c>
@@ -519,6 +528,9 @@
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>